<commit_message>
Create CreateSampleTeacher and both PrintTeacher functions
</commit_message>
<xml_diff>
--- a/Q&A/MusalaSoft Test.xlsx
+++ b/Q&A/MusalaSoft Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Musala-Soft-project\Q&amp;A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB14655-4C8D-4C7B-898C-314E6157CA30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D23CBA5-DF45-42D6-8825-8127DF87B511}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -322,16 +322,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
@@ -343,11 +348,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="6" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="6"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Accent3" xfId="6" builtinId="37"/>
@@ -637,12 +637,12 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="36.7109375" bestFit="1" customWidth="1"/>
@@ -679,7 +679,7 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="11" t="s">
         <v>28</v>
       </c>
     </row>
@@ -696,7 +696,7 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -708,7 +708,7 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="13" t="s">
         <v>31</v>
       </c>
     </row>
@@ -725,14 +725,14 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="14"/>
     </row>
     <row r="6" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -747,7 +747,7 @@
       <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="10" t="s">
         <v>28</v>
       </c>
     </row>
@@ -764,7 +764,7 @@
       <c r="D8" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="8"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -779,14 +779,14 @@
       <c r="D9" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="8"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -798,7 +798,7 @@
       <c r="D11" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="7" t="s">
         <v>30</v>
       </c>
     </row>
@@ -809,14 +809,14 @@
       <c r="D12" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="12"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -828,7 +828,7 @@
       <c r="D14" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="8" t="s">
         <v>29</v>
       </c>
     </row>
@@ -839,14 +839,14 @@
       <c r="D15" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="6"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Start of Code Cleanup. Create Log.h and Log.cpp.
</commit_message>
<xml_diff>
--- a/Q&A/MusalaSoft Test.xlsx
+++ b/Q&A/MusalaSoft Test.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Musala-Soft-project\Q&amp;A\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC7A359-42BC-4173-9F9F-F697C65AF826}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
   <si>
     <t>Function</t>
   </si>
@@ -108,9 +109,6 @@
   </si>
   <si>
     <t>good job</t>
-  </si>
-  <si>
-    <t>Issue should be fixed! Pls test again</t>
   </si>
   <si>
     <t>CreateSampleStudents only creates the student! Use PrintStudent to display. The input should be two vectors with names that are automatically generated.</t>
@@ -171,11 +169,14 @@
 Позволяване дублиране на ролите
 Позволява невалидни имеили и имена с малка буква.</t>
   </si>
+  <si>
+    <t>I had to make a major overhaul on inputs and outputs, most function calls got changed in the proccess</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -376,7 +377,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -384,13 +385,10 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
@@ -408,11 +406,17 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -441,20 +445,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1226820</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>3497580</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>162908</xdr:rowOff>
+      <xdr:rowOff>538193</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -492,13 +502,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1607820</xdr:colOff>
+      <xdr:colOff>1604010</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>172684</xdr:rowOff>
+      <xdr:rowOff>180304</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -536,13 +552,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1766226</xdr:colOff>
+      <xdr:colOff>1729806</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>177809</xdr:rowOff>
+      <xdr:rowOff>183524</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -836,24 +858,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="92.33203125" customWidth="1"/>
-    <col min="6" max="6" width="36.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="92.28515625" customWidth="1"/>
+    <col min="6" max="6" width="142.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -866,11 +888,12 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -883,11 +906,11 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -900,9 +923,9 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -912,11 +935,11 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F4" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -929,16 +952,17 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="14"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -951,11 +975,11 @@
       <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -968,9 +992,9 @@
       <c r="D8" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -983,16 +1007,17 @@
       <c r="D9" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -1002,27 +1027,28 @@
       <c r="D11" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F11" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>21</v>
       </c>
       <c r="D12" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
@@ -1032,111 +1058,119 @@
       <c r="D14" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="F14" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="16"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="D18" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="E18" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>35</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E19" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" t="s">
         <v>40</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="F21" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="15" t="s">
+      <c r="E26" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="17" t="s">
         <v>43</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F4:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>